<commit_message>
added pictures of results graphs
</commit_message>
<xml_diff>
--- a/MASH-dev/AlecGeorgoff/Benchmarking/BM_outline/benchmarking_outline_2.xlsx
+++ b/MASH-dev/AlecGeorgoff/Benchmarking/BM_outline/benchmarking_outline_2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MASH-Main\MASH-dev\AlecGeorgoff\Benchmarking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MASH-Main\MASH-dev\AlecGeorgoff\Benchmarking\BM_outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="9470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,15 +224,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -244,33 +271,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -558,7 +558,7 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
@@ -652,7 +652,7 @@
       <c r="F2" s="1">
         <v>159371403</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1">
@@ -670,7 +670,7 @@
       <c r="L2" s="1">
         <v>159374722</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O2" s="1">
@@ -690,7 +690,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1">
         <v>500</v>
       </c>
@@ -706,7 +706,7 @@
       <c r="F3" s="1">
         <v>159371404</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="1">
         <v>5000</v>
       </c>
@@ -722,7 +722,7 @@
       <c r="L3" s="1">
         <v>159374723</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="25"/>
       <c r="O3" s="1">
         <v>500</v>
       </c>
@@ -740,7 +740,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="1">
         <v>500</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="F4" s="1">
         <v>159371405</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="1">
         <v>5000</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="L4" s="1">
         <v>159374724</v>
       </c>
-      <c r="N4" s="15"/>
+      <c r="N4" s="25"/>
       <c r="O4" s="1">
         <v>500</v>
       </c>
@@ -790,7 +790,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1">
         <v>500</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="F5" s="1">
         <v>159371406</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="1">
         <v>5000</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="L5" s="1">
         <v>159374725</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="25"/>
       <c r="O5" s="1">
         <v>500</v>
       </c>
@@ -840,7 +840,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2">
         <v>500</v>
       </c>
@@ -856,7 +856,7 @@
       <c r="F6" s="2">
         <v>159371407</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="2">
         <v>5000</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="L6" s="2">
         <v>159374726</v>
       </c>
-      <c r="N6" s="16"/>
+      <c r="N6" s="26"/>
       <c r="O6" s="2">
         <v>500</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
@@ -910,7 +910,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="1">
         <v>5000</v>
       </c>
@@ -928,7 +928,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1">
         <v>5000</v>
       </c>
@@ -976,7 +976,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="1">
         <v>5000</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="F10" s="1">
         <v>159374725</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="24" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
@@ -1010,7 +1010,7 @@
       <c r="L10" s="1">
         <v>159754607</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="24" t="s">
         <v>6</v>
       </c>
       <c r="O10" s="3">
@@ -1030,7 +1030,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="2">
         <v>5000</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="F11" s="2">
         <v>159374726</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="3">
         <v>50000</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="L11" s="1">
         <v>159754608</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="25"/>
       <c r="O11" s="3">
         <v>300</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="3">
@@ -1098,7 +1098,7 @@
       <c r="F12" s="1">
         <v>159754607</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="3">
         <v>50000</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="L12" s="1">
         <v>159754610</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="25"/>
       <c r="O12" s="3">
         <v>1000</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="3">
         <v>50000</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="F13" s="1">
         <v>159754608</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="4">
         <v>50000</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="L13" s="2">
         <v>159754612</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="3">
         <v>3000</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="3">
         <v>50000</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>159754610</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="N14" s="15"/>
+      <c r="N14" s="25"/>
       <c r="O14" s="3">
         <v>10000</v>
       </c>
@@ -1217,7 +1217,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="4">
         <v>50000</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>159754612</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="N15" s="16"/>
+      <c r="N15" s="26"/>
       <c r="O15" s="4">
         <v>30000</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="3">
@@ -1273,7 +1273,7 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="3">
         <v>300</v>
       </c>
@@ -1305,24 +1305,24 @@
       <c r="L17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="29" t="s">
+      <c r="P17" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="30" t="s">
+      <c r="Q17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="S17" s="30" t="s">
+      <c r="S17" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="3">
         <v>1000</v>
       </c>
@@ -1338,45 +1338,45 @@
       <c r="F18" s="1">
         <v>159752822</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="1">
-        <v>500</v>
-      </c>
-      <c r="I18" s="1">
-        <v>10</v>
-      </c>
-      <c r="J18" s="1">
-        <v>100</v>
-      </c>
-      <c r="K18" s="1">
-        <v>2</v>
-      </c>
-      <c r="L18" s="1">
-        <v>159371403</v>
-      </c>
-      <c r="N18" s="17" t="s">
+      <c r="H18" s="16">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="16">
+        <v>10</v>
+      </c>
+      <c r="J18" s="16">
+        <v>365</v>
+      </c>
+      <c r="K18" s="17">
+        <v>2</v>
+      </c>
+      <c r="L18" s="18">
+        <v>162313618</v>
+      </c>
+      <c r="N18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="16">
         <v>1000</v>
       </c>
-      <c r="P18" s="23">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="23">
-        <v>365</v>
-      </c>
-      <c r="R18" s="24">
-        <v>2</v>
-      </c>
-      <c r="S18" s="25">
+      <c r="P18" s="16">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>365</v>
+      </c>
+      <c r="R18" s="17">
+        <v>2</v>
+      </c>
+      <c r="S18" s="18">
         <v>162314631</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="3">
         <v>3000</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="F19" s="1">
         <v>159752823</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="3">
         <v>3000</v>
       </c>
@@ -1402,13 +1402,13 @@
       <c r="J19" s="3">
         <v>365</v>
       </c>
-      <c r="K19" s="26">
-        <v>2</v>
-      </c>
-      <c r="L19" s="27">
+      <c r="K19" s="19">
+        <v>2</v>
+      </c>
+      <c r="L19" s="20">
         <v>162313619</v>
       </c>
-      <c r="N19" s="15"/>
+      <c r="N19" s="25"/>
       <c r="O19" s="3">
         <v>3000</v>
       </c>
@@ -1418,15 +1418,15 @@
       <c r="Q19" s="3">
         <v>365</v>
       </c>
-      <c r="R19" s="26">
-        <v>2</v>
-      </c>
-      <c r="S19" s="27">
+      <c r="R19" s="19">
+        <v>2</v>
+      </c>
+      <c r="S19" s="20">
         <v>162314632</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="3">
         <v>10000</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="F20" s="1">
         <v>159752825</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="3">
         <v>10000</v>
       </c>
@@ -1452,13 +1452,13 @@
       <c r="J20" s="3">
         <v>365</v>
       </c>
-      <c r="K20" s="26">
-        <v>2</v>
-      </c>
-      <c r="L20" s="27">
+      <c r="K20" s="19">
+        <v>2</v>
+      </c>
+      <c r="L20" s="20">
         <v>162313620</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="25"/>
       <c r="O20" s="3">
         <v>10000</v>
       </c>
@@ -1468,15 +1468,15 @@
       <c r="Q20" s="3">
         <v>365</v>
       </c>
-      <c r="R20" s="26">
-        <v>2</v>
-      </c>
-      <c r="S20" s="27">
+      <c r="R20" s="19">
+        <v>2</v>
+      </c>
+      <c r="S20" s="20">
         <v>162314633</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="4">
         <v>30000</v>
       </c>
@@ -1492,7 +1492,7 @@
       <c r="F21" s="2">
         <v>159752827</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="3">
         <v>30000</v>
       </c>
@@ -1502,13 +1502,13 @@
       <c r="J21" s="3">
         <v>365</v>
       </c>
-      <c r="K21" s="26">
-        <v>2</v>
-      </c>
-      <c r="L21" s="27">
+      <c r="K21" s="19">
+        <v>2</v>
+      </c>
+      <c r="L21" s="20">
         <v>162313621</v>
       </c>
-      <c r="N21" s="15"/>
+      <c r="N21" s="25"/>
       <c r="O21" s="3">
         <v>30000</v>
       </c>
@@ -1518,33 +1518,33 @@
       <c r="Q21" s="3">
         <v>365</v>
       </c>
-      <c r="R21" s="26">
-        <v>2</v>
-      </c>
-      <c r="S21" s="27">
+      <c r="R21" s="19">
+        <v>2</v>
+      </c>
+      <c r="S21" s="20">
         <v>162314634</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="16">
         <v>1000</v>
       </c>
-      <c r="C22" s="23">
-        <v>10</v>
-      </c>
-      <c r="D22" s="23">
-        <v>365</v>
-      </c>
-      <c r="E22" s="24">
-        <v>2</v>
-      </c>
-      <c r="F22" s="25">
+      <c r="C22" s="16">
+        <v>10</v>
+      </c>
+      <c r="D22" s="16">
+        <v>365</v>
+      </c>
+      <c r="E22" s="17">
+        <v>2</v>
+      </c>
+      <c r="F22" s="18">
         <v>162313618</v>
       </c>
-      <c r="G22" s="15"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="3">
         <v>100000</v>
       </c>
@@ -1554,13 +1554,13 @@
       <c r="J22" s="3">
         <v>365</v>
       </c>
-      <c r="K22" s="26">
-        <v>2</v>
-      </c>
-      <c r="L22" s="27">
+      <c r="K22" s="19">
+        <v>2</v>
+      </c>
+      <c r="L22" s="20">
         <v>162313622</v>
       </c>
-      <c r="N22" s="15"/>
+      <c r="N22" s="25"/>
       <c r="O22" s="3">
         <v>100000</v>
       </c>
@@ -1570,15 +1570,15 @@
       <c r="Q22" s="3">
         <v>365</v>
       </c>
-      <c r="R22" s="26">
+      <c r="R22" s="19">
         <v>8</v>
       </c>
-      <c r="S22" s="27">
+      <c r="S22" s="20">
         <v>162314636</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="3">
         <v>3000</v>
       </c>
@@ -1588,13 +1588,13 @@
       <c r="D23" s="3">
         <v>365</v>
       </c>
-      <c r="E23" s="26">
-        <v>2</v>
-      </c>
-      <c r="F23" s="27">
+      <c r="E23" s="19">
+        <v>2</v>
+      </c>
+      <c r="F23" s="20">
         <v>162313619</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="3">
         <v>200000</v>
       </c>
@@ -1604,13 +1604,13 @@
       <c r="J23" s="3">
         <v>365</v>
       </c>
-      <c r="K23" s="26">
-        <v>2</v>
-      </c>
-      <c r="L23" s="27">
+      <c r="K23" s="19">
+        <v>2</v>
+      </c>
+      <c r="L23" s="20">
         <v>162313623</v>
       </c>
-      <c r="N23" s="15"/>
+      <c r="N23" s="25"/>
       <c r="O23" s="3">
         <v>200000</v>
       </c>
@@ -1620,15 +1620,15 @@
       <c r="Q23" s="3">
         <v>365</v>
       </c>
-      <c r="R23" s="26">
+      <c r="R23" s="19">
         <v>8</v>
       </c>
-      <c r="S23" s="27">
+      <c r="S23" s="20">
         <v>162314637</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="15"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="3">
         <v>10000</v>
       </c>
@@ -1638,13 +1638,13 @@
       <c r="D24" s="3">
         <v>365</v>
       </c>
-      <c r="E24" s="26">
-        <v>2</v>
-      </c>
-      <c r="F24" s="27">
+      <c r="E24" s="19">
+        <v>2</v>
+      </c>
+      <c r="F24" s="20">
         <v>162313620</v>
       </c>
-      <c r="G24" s="16"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="2">
         <v>300000</v>
       </c>
@@ -1657,10 +1657,10 @@
       <c r="K24" s="2">
         <v>2</v>
       </c>
-      <c r="L24" s="28">
+      <c r="L24" s="21">
         <v>162313624</v>
       </c>
-      <c r="N24" s="16"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="2">
         <v>300000</v>
       </c>
@@ -1673,12 +1673,12 @@
       <c r="R24" s="2">
         <v>8</v>
       </c>
-      <c r="S24" s="28">
+      <c r="S24" s="21">
         <v>162314638</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="3">
         <v>30000</v>
       </c>
@@ -1688,15 +1688,15 @@
       <c r="D25" s="3">
         <v>365</v>
       </c>
-      <c r="E25" s="26">
-        <v>2</v>
-      </c>
-      <c r="F25" s="27">
+      <c r="E25" s="19">
+        <v>2</v>
+      </c>
+      <c r="F25" s="20">
         <v>162313621</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="3">
         <v>100000</v>
       </c>
@@ -1706,15 +1706,15 @@
       <c r="D26" s="3">
         <v>365</v>
       </c>
-      <c r="E26" s="26">
-        <v>2</v>
-      </c>
-      <c r="F26" s="27">
+      <c r="E26" s="19">
+        <v>2</v>
+      </c>
+      <c r="F26" s="20">
         <v>162313622</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="3">
         <v>200000</v>
       </c>
@@ -1724,15 +1724,15 @@
       <c r="D27" s="3">
         <v>365</v>
       </c>
-      <c r="E27" s="26">
-        <v>2</v>
-      </c>
-      <c r="F27" s="27">
+      <c r="E27" s="19">
+        <v>2</v>
+      </c>
+      <c r="F27" s="20">
         <v>162313623</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2">
         <v>300000</v>
       </c>
@@ -1745,12 +1745,12 @@
       <c r="E28" s="2">
         <v>2</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="21">
         <v>162313624</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="3">
@@ -1765,12 +1765,12 @@
       <c r="E29" s="1">
         <v>2</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="15">
         <v>162314631</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="3">
         <v>3000</v>
       </c>
@@ -1783,12 +1783,12 @@
       <c r="E30" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="15">
         <v>162314632</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="18"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="3">
         <v>10000</v>
       </c>
@@ -1801,12 +1801,12 @@
       <c r="E31" s="1">
         <v>2</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="15">
         <v>162314633</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="3">
         <v>30000</v>
       </c>
@@ -1819,12 +1819,12 @@
       <c r="E32" s="1">
         <v>2</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="15">
         <v>162314634</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="3">
         <v>100000</v>
       </c>
@@ -1837,12 +1837,12 @@
       <c r="E33" s="1">
         <v>8</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="15">
         <v>162314636</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="3">
         <v>200000</v>
       </c>
@@ -1855,12 +1855,12 @@
       <c r="E34" s="1">
         <v>8</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="15">
         <v>162314637</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="1">
         <v>300000</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="E35" s="1">
         <v>8</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="15">
         <v>162314638</v>
       </c>
     </row>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="11">
@@ -1953,7 +1953,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="11">
         <v>500</v>
       </c>
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="11">
         <v>500</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="11">
         <v>500</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="12">
         <v>500</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="11">
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="11">
         <v>5000</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="11">
         <v>5000</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="11">
         <v>5000</v>
       </c>
@@ -2108,7 +2108,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="20"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="12">
         <v>5000</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="13">
@@ -2147,7 +2147,7 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="13">
         <v>50000</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="13">
         <v>50000</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="14">
         <v>50000</v>
       </c>
@@ -2204,7 +2204,7 @@
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="13">
@@ -2225,7 +2225,7 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="13">
         <v>300</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="13">
         <v>1000</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="13">
         <v>3000</v>
       </c>
@@ -2282,7 +2282,7 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="13">
         <v>10000</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="20"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="14">
         <v>30000</v>
       </c>
@@ -2320,7 +2320,7 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="3">
@@ -2335,12 +2335,12 @@
       <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="15">
         <v>162313618</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="18"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="3">
         <v>3000</v>
       </c>
@@ -2353,12 +2353,12 @@
       <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="15">
         <v>162313619</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="3">
         <v>10000</v>
       </c>
@@ -2371,12 +2371,12 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="15">
         <v>162313620</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="18"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="3">
         <v>30000</v>
       </c>
@@ -2389,12 +2389,12 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="15">
         <v>162313621</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="18"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="3">
         <v>100000</v>
       </c>
@@ -2407,12 +2407,12 @@
       <c r="E26" s="1">
         <v>2</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="15">
         <v>162313622</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="18"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="3">
         <v>200000</v>
       </c>
@@ -2425,12 +2425,12 @@
       <c r="E27" s="1">
         <v>2</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="15">
         <v>162313623</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="18"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="1">
         <v>300000</v>
       </c>
@@ -2443,15 +2443,15 @@
       <c r="E28" s="1">
         <v>2</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="15">
         <v>162313624</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F29" s="22"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="3">
@@ -2466,12 +2466,12 @@
       <c r="E30" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="15">
         <v>162314631</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="18"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="3">
         <v>3000</v>
       </c>
@@ -2484,12 +2484,12 @@
       <c r="E31" s="1">
         <v>2</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="15">
         <v>162314632</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="3">
         <v>10000</v>
       </c>
@@ -2502,12 +2502,12 @@
       <c r="E32" s="1">
         <v>2</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="15">
         <v>162314633</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="3">
         <v>30000</v>
       </c>
@@ -2520,12 +2520,12 @@
       <c r="E33" s="1">
         <v>2</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="15">
         <v>162314634</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="3">
         <v>100000</v>
       </c>
@@ -2538,12 +2538,12 @@
       <c r="E34" s="1">
         <v>8</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="15">
         <v>162314636</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="3">
         <v>200000</v>
       </c>
@@ -2556,12 +2556,12 @@
       <c r="E35" s="1">
         <v>8</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="15">
         <v>162314637</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="1">
         <v>300000</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="E36" s="1">
         <v>8</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="15">
         <v>162314638</v>
       </c>
     </row>

</xml_diff>